<commit_message>
pridanie textov do wordu
</commit_message>
<xml_diff>
--- a/DP/Tabulky.xlsx
+++ b/DP/Tabulky.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klein\Desktop\Diplomova-Praca\DP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9FA5DEA-BD16-4563-BB06-11CCF699D058}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933D6A95-7C1B-4D2A-933C-9A3E7BCE2630}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F9C9A39A-61D2-4D80-B3D9-FF61168FCDAD}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{F9C9A39A-61D2-4D80-B3D9-FF61168FCDAD}"/>
   </bookViews>
   <sheets>
     <sheet name="GPI" sheetId="1" r:id="rId1"/>
     <sheet name="Frekvencny rozsah" sheetId="2" r:id="rId2"/>
+    <sheet name="pásmo 434 MHz" sheetId="3" r:id="rId3"/>
+    <sheet name="pásmo 868 MHz" sheetId="4" r:id="rId4"/>
+    <sheet name="pásmo 2400 MHz" sheetId="6" r:id="rId5"/>
+    <sheet name="RF modul" sheetId="7" r:id="rId6"/>
+    <sheet name="Bluetooth" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="192">
   <si>
     <t>Pin No.</t>
   </si>
@@ -185,13 +190,457 @@
   </si>
   <si>
     <t>Tally / GPI 2</t>
+  </si>
+  <si>
+    <t>Využitie</t>
+  </si>
+  <si>
+    <t>Dodatočné parametre
+(šírka kanálov a/alebo pravidlá
+prístupu a obsadenia kanálov)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iné obmedzenia
+používania </t>
+  </si>
+  <si>
+    <t>Maximálny povolený výkon</t>
+  </si>
+  <si>
+    <t>Frekvenčné pásmo</t>
+  </si>
+  <si>
+    <t>433,050 - 434,040 MHz
+(pásmo 44b v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>433,050 - 434,040 MHz
+(pásmo 44a v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>434,040 - 434,790 MHz
+(pásmo 45a v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>434,040 - 434,790 MHz
+(pásmo 45b v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>434,040 - 434,790 MHz                                         (pásmo 45c v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>e.r.p. 10 mW</t>
+  </si>
+  <si>
+    <t>Hlasové aplikácie sú povolené za použitia techník na zmiernenie rušenia.</t>
+  </si>
+  <si>
+    <t>Maximálny pracovný cyklus &lt; 10 % (3)</t>
+  </si>
+  <si>
+    <t>Audio a video aplikácie sú vylúčené.</t>
+  </si>
+  <si>
+    <t>Analógové audio aplikácie, okrem hlasových, sú vylúčené. Analógové video aplikácie sú vylúčené.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pracovný cyklus 100% (3). Šírka kanála je maximálne 25 kHz. Hlasové aplikácie sú povolené za použitia techník na zníženie rušenia. </t>
+  </si>
+  <si>
+    <t>Nešpecifikované SRD</t>
+  </si>
+  <si>
+    <t>Na prístup k frekvenčnému spektru a na zmiernenie rušenia sa musia použiť techniky rovnako účinné, ako techniky opísané v harmonizovaných normách prijatých podľa smernice 2014/53/EÚ. Šírka pásma ≤ 200 kHz. Pre prístupové body siete je pracovný cyklus ≤ 10 %. V ostatných prípadoch je pracovný cyklus ≤ 2,5 % ( 3 ).</t>
+  </si>
+  <si>
+    <t>Uvedené podmienky používania je možné uplatniť len pre dátové siete.</t>
+  </si>
+  <si>
+    <t>Analógové video aplikácie sú vylúčené.</t>
+  </si>
+  <si>
+    <t>e.r.p. 500 mW</t>
+  </si>
+  <si>
+    <t>Na prístup k frekvenčnému spektru a na zmiernenie rušenia sa musia použiť techniky rovnako účinné, ako techniky opísané v harmonizovaných normách prijatých podľa smernice 2014/53/EÚ. Alternatívne je možné použiť pracovný cyklus 10% ( 3 )</t>
+  </si>
+  <si>
+    <t>e.r.p. 5 mW</t>
+  </si>
+  <si>
+    <t>Hlasové aplikácie sú povolené za použitia vyspelých techník na zmiernenie rušenia.</t>
+  </si>
+  <si>
+    <t>RLAN</t>
+  </si>
+  <si>
+    <t>Tento súbor podmienok používania sa vzťahuje len na širokopásmové zariadenia s krátkym dosahom v bezdrôtových dátových sieťach. (5 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> e.r.p.  25 mW</t>
+  </si>
+  <si>
+    <t>865,000 - 868,000 MHz                                     (pásmo 47 v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">868,000 - 868,600 MHz                                   (pásmo 48 v (EU) 2017/1483   </t>
+  </si>
+  <si>
+    <t>868,700 - 869,200 MHz                                    (pásmo 50 v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>Analógové audio aplikácie okrem hlasových sú vylúčené. Analógové video aplikácie sú vylúčené.</t>
+  </si>
+  <si>
+    <t>869,700 - 870,000 MHz                                    (pásmo 56b v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>863-868 MHz                                                   (pásmo 84 v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>Na prístup k frekvenčnému spektru a na zmiernenie rušenia sa musia použiť techniky rovnako účinné ako techniky opísané v harmonizovaných normách prijatých podľa smernice 2014/53/EÚ. 
+Šírka pásma: ≤ 1 MHz. 
+Pracovný cyklus(4 ): ≤ 10 %
+ pre prístupové body siete. 
+Pracovný cyklus: ≤ 2,8 % v ostatných prípadoch.</t>
+  </si>
+  <si>
+    <t>869,700 - 870,000 MHz 
+(pásmo 56a v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>Na prístup k frekvenčnému spektru a na zmiernenie rušenia sa musia použiť techniky rovnako účinné, ako techniky opísané v harmonizovaných normách prijatých podľa smernice 2014/53/EÚ. 
+Alternatívne je možné použiť pracovný cyklus 1% ( 3 ).</t>
+  </si>
+  <si>
+    <t>e.r.p. 1 mW
+ a max. výkonová hustota
+ -13 dBm/10kHz (5) pri modulácii so šírkou pásma nad 250 kHz</t>
+  </si>
+  <si>
+    <t>863,000 - 865,000 MHz 
+(pásmo 46a v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>869,400 - 869,650 MHz
+ (pásmo 54 v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>865,000 - 868,000 MHz 
+(pásmo 47b v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2,400 - 2,4835 GHz
+ (pásmo 57a v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>e.i.r.p. 10 mW</t>
+  </si>
+  <si>
+    <t>max. 100 mW e.i.r.p.( 6 ) len pre moduláciu FHSS s maximálnou spektrálnou výkonovou hustotou 100 mW/100 kHz e.i.r.p. Pre modulácie iné ako FHSS je maximálna spektrálna výkonová hustota obmedzená na 10 mW/1 MHz e.i.r.p.</t>
+  </si>
+  <si>
+    <t>Na prístup k frekvenčnému spektru a na zmiernenie rušenia sa musia použiť techniky rovnako účinné ako techniky opísané v harmonizovaných normách prijatých podľa smernice 2014/53/EÚ.</t>
+  </si>
+  <si>
+    <t>2,400 - 2,4835 GHz
+(pásmo 57c v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>2 483,5 - 2 500 MHz (pásmo 59a v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>1 mW</t>
+  </si>
+  <si>
+    <t>Na prístup k frekvenčnému spektru a na zmiernenie rušenia sa musia použiť techniky rovnako účinné ako techniky opísané v harmonizovaných normách prijatých podľa smernice 2014/53/EÚ. Maximálny pracovný cyklus 10 %. ( 1 ) Kanálová šírka: ≤ 3 MHz.</t>
+  </si>
+  <si>
+    <t>MBAND</t>
+  </si>
+  <si>
+    <t>Len pre systémy získavania
+zdravotníckych údajov
+(Medical Body Area Network
+System – MBANS).
+Na používanie vo vnútorných
+priestoroch v rámci zariadení
+zdravotnej starostlivosti.
+(Indoor only)</t>
+  </si>
+  <si>
+    <t>10 mW</t>
+  </si>
+  <si>
+    <t>2 483,5 - 2 500 MHz (pásmo 59b v (EU) 2017/1483)</t>
+  </si>
+  <si>
+    <t>Na prístup k frekvenčnému spektru a na zmiernenie rušenia sa musia použiť techniky rovnako účinné ako techniky opísané v harmonizovaných normách prijatých podľa smernice 2014/53/EÚ. Maximálny pracovný cyklus 2 %. ( 1 ) Kanálová šírka: ≤ 3 MHz.</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Hodnota</t>
+  </si>
+  <si>
+    <t>Popis</t>
+  </si>
+  <si>
+    <t>Pracovná frekvencia</t>
+  </si>
+  <si>
+    <t>Vysielaci výkon</t>
+  </si>
+  <si>
+    <t>Citlivosť príjmača</t>
+  </si>
+  <si>
+    <t>Vzdušná dátová rýchlosť</t>
+  </si>
+  <si>
+    <t>Dosah</t>
+  </si>
+  <si>
+    <t>2400~2518 MHz</t>
+  </si>
+  <si>
+    <t>10~20 dBm</t>
+  </si>
+  <si>
+    <t>-102 dBm</t>
+  </si>
+  <si>
+    <t>250k~2Mbps</t>
+  </si>
+  <si>
+    <t>2500m</t>
+  </si>
+  <si>
+    <t>základné nastavenie: 2400 MHz</t>
+  </si>
+  <si>
+    <t>základné nastavenie: 20 dBm (100 mW)</t>
+  </si>
+  <si>
+    <t>pri prenosovej rýchlosti 250 kbps</t>
+  </si>
+  <si>
+    <t>základné nastavenie: 250 kbps</t>
+  </si>
+  <si>
+    <t>Na otvorenom priestranstve, maximálny výkonom, zosilnenie antény 5dBi, prenosová rýchlosť 250kbps</t>
+  </si>
+  <si>
+    <t>Prídavné funkcie</t>
+  </si>
+  <si>
+    <t>FEC, FHSS</t>
+  </si>
+  <si>
+    <t>Konektror antény</t>
+  </si>
+  <si>
+    <t>SMA-K</t>
+  </si>
+  <si>
+    <t>Komunikačné rozhranie</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>Baudrate: 1200~11520, základný - 9600</t>
+  </si>
+  <si>
+    <t>Zásobník</t>
+  </si>
+  <si>
+    <t>256 bajtov</t>
+  </si>
+  <si>
+    <t>Elektronické  parametre</t>
+  </si>
+  <si>
+    <t>Min.</t>
+  </si>
+  <si>
+    <t>Typ.</t>
+  </si>
+  <si>
+    <t>Max.</t>
+  </si>
+  <si>
+    <t>Napájacie napätie</t>
+  </si>
+  <si>
+    <t>Komunikačná úroveń</t>
+  </si>
+  <si>
+    <t>Príjamcí prúd</t>
+  </si>
+  <si>
+    <t>Spánok</t>
+  </si>
+  <si>
+    <t>Operačná teplota</t>
+  </si>
+  <si>
+    <t>Operačná vlhkosť</t>
+  </si>
+  <si>
+    <t>℃</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>μA</t>
+  </si>
+  <si>
+    <t>mA</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napájacie napätie </t>
+  </si>
+  <si>
+    <t>Vysielaci prúd (20dBm)</t>
+  </si>
+  <si>
+    <t>Smer</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Funkcia</t>
+  </si>
+  <si>
+    <t>8, 9, 10</t>
+  </si>
+  <si>
+    <t>M0</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>RXD</t>
+  </si>
+  <si>
+    <t>TXD</t>
+  </si>
+  <si>
+    <t>AUX</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>UART RX  konektor</t>
+  </si>
+  <si>
+    <t>UART TX  konektor</t>
+  </si>
+  <si>
+    <t>Zem</t>
+  </si>
+  <si>
+    <t>Napíjacie napätie</t>
+  </si>
+  <si>
+    <t>Konektor generuje impulz pri prichádzajúcich dátach</t>
+  </si>
+  <si>
+    <t>Fixačné otvory</t>
+  </si>
+  <si>
+    <t>M0, M1 slúžia na prepínanie módov modulu</t>
+  </si>
+  <si>
+    <t>Parametre</t>
+  </si>
+  <si>
+    <t>Bluetooth technológia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v2.0</t>
+  </si>
+  <si>
+    <t>4-6 V</t>
+  </si>
+  <si>
+    <t>Komunikačná úroveň</t>
+  </si>
+  <si>
+    <t>3,3 V</t>
+  </si>
+  <si>
+    <t>Módy</t>
+  </si>
+  <si>
+    <t>Master, Slave, Master/Slave</t>
+  </si>
+  <si>
+    <t>Rozhranie</t>
+  </si>
+  <si>
+    <t>Baudrate: 9600 - 460800</t>
+  </si>
+  <si>
+    <t>Anténa</t>
+  </si>
+  <si>
+    <t>integrovaná na DPS</t>
+  </si>
+  <si>
+    <t>možné nastaviť</t>
+  </si>
+  <si>
+    <t>Prenosová rýchlosť</t>
+  </si>
+  <si>
+    <t>2Mbps - 3Mbps</t>
+  </si>
+  <si>
+    <t>max. 30 mA</t>
+  </si>
+  <si>
+    <t>Vysielací prúd</t>
+  </si>
+  <si>
+    <t>pri výkone 6 dBm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + EDR</t>
+  </si>
+  <si>
+    <t>max. 6 dBm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,8 +663,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,8 +705,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -381,11 +864,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,73 +1065,223 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -811,32 +1615,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="31" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1096,150 +1900,1079 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0389589E-5265-472E-93CD-5CC816E74C62}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="16"/>
-    <col min="2" max="2" width="24.85546875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="33" style="16" customWidth="1"/>
-    <col min="4" max="16384" width="28.85546875" style="16"/>
+    <col min="1" max="1" width="28.85546875" style="12"/>
+    <col min="2" max="2" width="24.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="33" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="28.85546875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:3" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="16">
         <v>6780</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="16">
         <v>13560</v>
       </c>
-      <c r="C3" s="25"/>
-    </row>
-    <row r="4" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="16">
         <v>27120</v>
       </c>
-      <c r="C4" s="25"/>
-    </row>
-    <row r="5" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="25"/>
-    </row>
-    <row r="6" spans="1:3" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="C5" s="21"/>
+    </row>
+    <row r="6" spans="1:3" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="15">
         <v>915</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="15">
         <v>2450</v>
       </c>
-      <c r="C8" s="25"/>
-    </row>
-    <row r="9" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="15">
         <v>5800</v>
       </c>
-      <c r="C9" s="25"/>
-    </row>
-    <row r="10" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="15">
         <v>24125</v>
       </c>
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="15">
+        <v>61250</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="15">
+        <v>122500</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="24">
+        <v>245000</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="14" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63017BE-BEBD-49BF-AC79-6C848985FC25}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="22" style="27" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="23" style="27" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="27" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
+    </row>
+    <row r="4" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="57"/>
+    </row>
+    <row r="6" spans="1:5" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D4E9A0-AE1C-455B-95ED-E427ADE98576}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" style="38" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="12" style="38" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="38" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="38"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="56"/>
+      <c r="E10" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="D3:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF34C18-C8FE-405D-8060-35F3B35010E9}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="27" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="37"/>
+    </row>
+    <row r="4" spans="1:5" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D4:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E1549F-EED8-4B73-ABAA-5DB7BB10F990}">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="20" style="28" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" style="28" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="28"/>
+    <col min="5" max="5" width="22.5703125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="28" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="28" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="28"/>
+    <col min="11" max="11" width="8" style="28" customWidth="1"/>
+    <col min="12" max="12" width="7" style="28" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="28" customWidth="1"/>
+    <col min="14" max="14" width="49.5703125" style="28" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="67"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="59"/>
+      <c r="G13" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" s="28">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H14" s="28">
+        <v>5</v>
+      </c>
+      <c r="I14" s="28">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="H15" s="28">
+        <v>3.3</v>
+      </c>
+      <c r="I15" s="28">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="28">
+        <v>100</v>
+      </c>
+      <c r="H16" s="28">
+        <v>110</v>
+      </c>
+      <c r="I16" s="28">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E17" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="28">
+        <v>20.5</v>
+      </c>
+      <c r="H17" s="28">
+        <v>21.5</v>
+      </c>
+      <c r="I17" s="28">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E18" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="G18" s="28">
+        <v>23.8</v>
+      </c>
+      <c r="H18" s="28">
+        <v>24.8</v>
+      </c>
+      <c r="I18" s="28">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E19" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="28">
+        <v>10</v>
+      </c>
+      <c r="H19" s="28">
+        <v>60</v>
+      </c>
+      <c r="I19" s="28">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" s="28">
+        <v>-40</v>
+      </c>
+      <c r="H20" s="28">
+        <v>20</v>
+      </c>
+      <c r="I20" s="28">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="L21" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="M21" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="N21" s="73" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="K22" s="68">
+        <v>1</v>
+      </c>
+      <c r="L22" s="69" t="s">
+        <v>156</v>
+      </c>
+      <c r="M22" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="N22" s="70" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="K23" s="63">
+        <v>2</v>
+      </c>
+      <c r="L23" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="M23" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="N23" s="64"/>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="K24" s="63">
+        <v>3</v>
+      </c>
+      <c r="L24" s="62" t="s">
+        <v>158</v>
+      </c>
+      <c r="M24" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="N24" s="22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="K25" s="63">
+        <v>4</v>
+      </c>
+      <c r="L25" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="M25" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="K26" s="63">
+        <v>5</v>
+      </c>
+      <c r="L26" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="M26" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="N26" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="K27" s="63">
+        <v>6</v>
+      </c>
+      <c r="L27" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="M27" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="K28" s="63">
+        <v>7</v>
+      </c>
+      <c r="L28" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="M28" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="N28" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="L29" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="M29" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="N29" s="67" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="N22:N23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FE92F6-BD3C-4F56-A3B8-137C0A2C8962}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="21" style="13" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="79" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="81" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="78" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="21"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="15">
+        <v>3</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>183</v>
+      </c>
       <c r="C10" s="25"/>
     </row>
-    <row r="11" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="19">
-        <v>61250</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="19">
-        <v>122500</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="28">
-        <v>245000</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>